<commit_message>
operaciones de tipos de dato
</commit_message>
<xml_diff>
--- a/Documentación/Wogawg-Elementos-del-Lenguaje.xlsx
+++ b/Documentación/Wogawg-Elementos-del-Lenguaje.xlsx
@@ -1890,6 +1890,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2480,10 +2484,10 @@
   <dimension ref="A2:BZ99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8204,6 +8208,10 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="11">
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="BJ3:BN3"/>
     <mergeCell ref="BP3:BT3"/>
     <mergeCell ref="BV3:BZ3"/>
     <mergeCell ref="T3:X3"/>
@@ -8211,10 +8219,6 @@
     <mergeCell ref="AR3:AV3"/>
     <mergeCell ref="AX3:BB3"/>
     <mergeCell ref="BD3:BH3"/>
-    <mergeCell ref="I3:O3"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="BJ3:BN3"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>